<commit_message>
update Diccionario de datos
</commit_message>
<xml_diff>
--- a/DicDatos/Diccionario de Datos.xlsx
+++ b/DicDatos/Diccionario de Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desarrollo 6\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desarrollo 6\Desktop\INFORME REPARACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4541836F-5076-4939-973B-06ECB61F44DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54ABBBD-B4C6-42CC-B745-6045261E85DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBAC981C-1C88-48D0-B52C-ACDC5499E605}"/>
+    <workbookView xWindow="25410" yWindow="705" windowWidth="21990" windowHeight="13395" xr2:uid="{CBAC981C-1C88-48D0-B52C-ACDC5499E605}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="194">
   <si>
     <t>asdas</t>
   </si>
@@ -436,13 +436,390 @@
   </si>
   <si>
     <t>tbcarunidad</t>
+  </si>
+  <si>
+    <t>CREATE TABLE tbdiaggen(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    nIdDiag bigint unsigned primary key not  null auto_increment,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cCveMec varchar(10) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cCveRea varchar(10) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cCveSup varchar(10) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cDesCar varchar(100) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cDesTras varchar(100) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cMcaMot  varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cObsDiag varchar(500) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cTipCar varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cDesHP int(10) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   dtFecReg varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   dtHorReg varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cDesFall varchar(500) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nCveEmp varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nCveSrv varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nIdeUni varchar(10) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cTipMot varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nModUni int(10) not null</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE tbdiagdet(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    nIntDiag bigint unsigned primary key not null auto_increment,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    nFotDiag int not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cNomDiag varchar(500) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cObsDiag varchar(500) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    nIdDiag bigint unsigned not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    foreign key (nIdDiag) references tbDiagGen(nIdDiag) on delete cascade on update cascade</t>
+  </si>
+  <si>
+    <t>create table tbCarUnidad</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nCveReg int not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nIdeUni int not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nCveSrv int not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nCveEmpPer int not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nCveEmp int not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cCveUniAnt varchar(10) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cCveUni varchar(10) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   dtFecAdq DateTime not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cDesZon varchar(30) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cCodRut varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nEdoUni tinyint not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nModUni int not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cSerUni varchar(100) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cMotor varchar(100) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cMcaMot varchar(100) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cDesHP varchar(20) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cDesCar varchar(150) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cTipCar varchar(150) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PRIMARY KEY (nCveReg)</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <r>
+      <t>CREATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> `user` (</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  `id` int(11) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  `username` varchar(255) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  `password` varchar(255) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  `role` varchar(255) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  `createdAt` </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>datetime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(6) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> DEFAULT CURRENT_TIMESTAMP(6),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  `updateAT` </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>datetime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(6) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> DEFAULT CURRENT_TIMESTAMP(6),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  `name` varchar(100) DEFAULT </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NULL</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +833,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -478,7 +868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -547,11 +937,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,19 +1058,38 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,6 +1099,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,6 +1347,218 @@
           <a:solidFill>
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>27609</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>151848</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>676413</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>110435</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto de flecha 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89CBCB88-5003-012D-EB51-A54563A81D26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="19795435" y="345109"/>
+          <a:ext cx="6073913" cy="151848"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>745435</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>138043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>676413</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>124239</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector recto de flecha 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855AD584-073F-F05A-FAF7-06C46EBA41E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10311848" y="1684130"/>
+          <a:ext cx="690217" cy="565979"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>427934</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>179457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>524565</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165652</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto de flecha 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{392F8525-9E7C-AC40-0220-3F98B3707960}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6957391" y="5397500"/>
+          <a:ext cx="96631" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>27609</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>96630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Conector recto de flecha 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AE66D11-BBF7-B26F-0EA9-BB9D4DC5D295}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11885543" y="3561522"/>
+          <a:ext cx="7150653" cy="13804"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -1126,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E724CA90-887C-4522-B293-7D05F88ADE74}">
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,16 +1891,17 @@
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="24" max="24" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>67</v>
       </c>
@@ -1157,8 +1911,11 @@
       <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z2" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1222,8 +1979,11 @@
       <c r="V3" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z3" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1287,8 +2047,11 @@
       <c r="V4" s="1">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z4" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1352,8 +2115,11 @@
       <c r="V5" s="1">
         <v>2021</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z5" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1417,8 +2183,11 @@
       <c r="V6" s="1">
         <v>2016</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z6" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1482,8 +2251,11 @@
       <c r="V7" s="1">
         <v>2017</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z7" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1493,8 +2265,11 @@
       <c r="C8" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z8" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1504,8 +2279,21 @@
       <c r="C9" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L9" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="15"/>
+      <c r="Z9" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1515,8 +2303,15 @@
       <c r="C10" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L10" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="S10" s="17"/>
+      <c r="Z10" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1526,8 +2321,15 @@
       <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L11" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="S11" s="17"/>
+      <c r="Z11" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1552,8 +2354,15 @@
       <c r="J12" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L12" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="S12" s="17"/>
+      <c r="Z12" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1578,8 +2387,15 @@
       <c r="J13" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L13" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="S13" s="17"/>
+      <c r="Z13" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1604,8 +2420,15 @@
       <c r="J14" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L14" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="S14" s="17"/>
+      <c r="Z14" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1615,8 +2438,20 @@
       <c r="C15" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L15" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="S15" s="17"/>
+      <c r="V15" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="W15" s="33"/>
+      <c r="X15" s="34"/>
+      <c r="Z15" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1626,8 +2461,26 @@
       <c r="C16" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="19"/>
+      <c r="V16" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="W16" s="36"/>
+      <c r="X16" s="37"/>
+      <c r="Z16" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1637,8 +2490,16 @@
       <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V17" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="W17" s="36"/>
+      <c r="X17" s="37"/>
+      <c r="Z17" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1648,8 +2509,16 @@
       <c r="C18" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V18" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="W18" s="36"/>
+      <c r="X18" s="37"/>
+      <c r="Z18" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1680,8 +2549,16 @@
       <c r="L19" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V19" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="W19" s="36"/>
+      <c r="X19" s="37"/>
+      <c r="Z19" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1703,20 +2580,28 @@
       <c r="I20" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="6">
         <v>45000.77480240741</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <v>45000.77480240741</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
+      <c r="V20" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="W20" s="36"/>
+      <c r="X20" s="37"/>
+      <c r="Z20" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="F21" s="1">
         <v>45</v>
       </c>
@@ -1729,24 +2614,37 @@
       <c r="I21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>45035.447672638889</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>45035.447672638889</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="V21" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="W21" s="36"/>
+      <c r="X21" s="37"/>
+      <c r="Z21" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="V22" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="W22" s="36"/>
+      <c r="X22" s="37"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
@@ -1756,8 +2654,13 @@
       <c r="C23" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V23" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="W23" s="39"/>
+      <c r="X23" s="40"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -1768,7 +2671,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -1779,7 +2682,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -1847,7 +2750,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1878,7 +2781,7 @@
       <c r="L27" s="1">
         <v>500</v>
       </c>
-      <c r="M27" s="8">
+      <c r="M27" s="7">
         <v>42591</v>
       </c>
       <c r="N27" s="1" t="s">
@@ -1915,10 +2818,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
       <c r="F28" s="1">
         <v>2</v>
       </c>
@@ -1940,7 +2843,7 @@
       <c r="L28" s="1">
         <v>501</v>
       </c>
-      <c r="M28" s="8">
+      <c r="M28" s="7">
         <v>42612</v>
       </c>
       <c r="N28" s="1" t="s">
@@ -1977,14 +2880,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>67</v>
       </c>
@@ -1995,7 +2898,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
@@ -2006,7 +2909,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -2017,7 +2920,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -2028,7 +2931,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
@@ -2038,8 +2941,13 @@
       <c r="C34" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F34" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
@@ -2049,8 +2957,12 @@
       <c r="C35" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F35" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
@@ -2060,8 +2972,13 @@
       <c r="C36" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F36" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36" s="21"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>86</v>
       </c>
@@ -2071,20 +2988,32 @@
       <c r="C37" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+      <c r="F37" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F38" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="21"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="24"/>
+      <c r="C39" s="28"/>
+      <c r="F39" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>67</v>
       </c>
@@ -2094,8 +3023,13 @@
       <c r="C40" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F40" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G40" s="21"/>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>100</v>
       </c>
@@ -2105,8 +3039,13 @@
       <c r="C41" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F41" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" s="21"/>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -2116,8 +3055,13 @@
       <c r="C42" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F42" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="G42" s="21"/>
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
@@ -2127,8 +3071,13 @@
       <c r="C43" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F43" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="G43" s="21"/>
+      <c r="H43" s="22"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>104</v>
       </c>
@@ -2138,8 +3087,13 @@
       <c r="C44" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F44" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="G44" s="21"/>
+      <c r="H44" s="22"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -2149,8 +3103,13 @@
       <c r="C45" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F45" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="G45" s="21"/>
+      <c r="H45" s="22"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>107</v>
       </c>
@@ -2160,8 +3119,13 @@
       <c r="C46" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F46" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="G46" s="21"/>
+      <c r="H46" s="22"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>109</v>
       </c>
@@ -2171,8 +3135,13 @@
       <c r="C47" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F47" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="G47" s="21"/>
+      <c r="H47" s="22"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>111</v>
       </c>
@@ -2182,8 +3151,13 @@
       <c r="C48" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F48" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="G48" s="21"/>
+      <c r="H48" s="22"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>114</v>
       </c>
@@ -2193,8 +3167,13 @@
       <c r="C49" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F49" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G49" s="21"/>
+      <c r="H49" s="22"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>117</v>
       </c>
@@ -2204,8 +3183,13 @@
       <c r="C50" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F50" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G50" s="21"/>
+      <c r="H50" s="22"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>119</v>
       </c>
@@ -2215,8 +3199,13 @@
       <c r="C51" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F51" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G51" s="21"/>
+      <c r="H51" s="22"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>41</v>
       </c>
@@ -2226,8 +3215,13 @@
       <c r="C52" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F52" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="G52" s="21"/>
+      <c r="H52" s="22"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>122</v>
       </c>
@@ -2237,8 +3231,13 @@
       <c r="C53" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F53" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="G53" s="21"/>
+      <c r="H53" s="22"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>124</v>
       </c>
@@ -2248,8 +3247,13 @@
       <c r="C54" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F54" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="G54" s="21"/>
+      <c r="H54" s="22"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
@@ -2259,8 +3263,13 @@
       <c r="C55" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F55" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="G55" s="21"/>
+      <c r="H55" s="22"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>40</v>
       </c>
@@ -2270,8 +3279,13 @@
       <c r="C56" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F56" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="19"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>33</v>
       </c>
@@ -2282,7 +3296,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>28</v>
       </c>
@@ -2293,7 +3307,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>32</v>
       </c>
@@ -2305,11 +3319,32 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="25">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A39:C39"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:C21">
     <cfRule type="dataBar" priority="4">
@@ -2368,7 +3403,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>